<commit_message>
modified domain xlsx file
</commit_message>
<xml_diff>
--- a/domain1.xlsx
+++ b/domain1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="893">
   <si>
     <t>p.s.360.cn</t>
   </si>
@@ -2632,6 +2632,74 @@
   </si>
   <si>
     <t>quanguo.58.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hz.58.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tj.58.com</t>
+  </si>
+  <si>
+    <t>infotopweb.union.vip.58.com</t>
+  </si>
+  <si>
+    <t>su.58.com</t>
+  </si>
+  <si>
+    <t>lieche.58.com</t>
+  </si>
+  <si>
+    <t>nj.58.com</t>
+  </si>
+  <si>
+    <t>dg.58.com</t>
+  </si>
+  <si>
+    <t>dl.58.com</t>
+  </si>
+  <si>
+    <t>hrb.58.com</t>
+  </si>
+  <si>
+    <t>chefenqi.58.com</t>
+  </si>
+  <si>
+    <t>sjz.58.com</t>
+  </si>
+  <si>
+    <t>weizhang.58.com</t>
+  </si>
+  <si>
+    <t>hshi.58.com</t>
+  </si>
+  <si>
+    <t>caipiao.58.com</t>
+  </si>
+  <si>
+    <t>epost.58.com</t>
+  </si>
+  <si>
+    <t>xa.58.com</t>
+  </si>
+  <si>
+    <t>cha.58.com</t>
+  </si>
+  <si>
+    <t>cq.58.com</t>
+  </si>
+  <si>
+    <t>ez.58.com</t>
+  </si>
+  <si>
+    <t>sou.58.com</t>
+  </si>
+  <si>
+    <t>cs.58.com</t>
+  </si>
+  <si>
+    <t>jn.58.com</t>
   </si>
 </sst>
 </file>
@@ -2956,10 +3024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B804"/>
+  <dimension ref="A1:B826"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A759" workbookViewId="0">
-      <selection activeCell="D771" sqref="D771"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9400,6 +9468,182 @@
         <v>788</v>
       </c>
     </row>
+    <row r="805" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A805" t="s">
+        <v>871</v>
+      </c>
+      <c r="B805" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="806" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A806" t="s">
+        <v>872</v>
+      </c>
+      <c r="B806" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="807" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A807" t="s">
+        <v>873</v>
+      </c>
+      <c r="B807" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="808" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A808" t="s">
+        <v>874</v>
+      </c>
+      <c r="B808" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="809" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A809" t="s">
+        <v>875</v>
+      </c>
+      <c r="B809" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A810" t="s">
+        <v>876</v>
+      </c>
+      <c r="B810" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="811" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A811" t="s">
+        <v>877</v>
+      </c>
+      <c r="B811" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A812" t="s">
+        <v>878</v>
+      </c>
+      <c r="B812" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="813" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A813" t="s">
+        <v>879</v>
+      </c>
+      <c r="B813" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A814" t="s">
+        <v>880</v>
+      </c>
+      <c r="B814" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A815" t="s">
+        <v>881</v>
+      </c>
+      <c r="B815" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="816" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A816" t="s">
+        <v>882</v>
+      </c>
+      <c r="B816" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A817" t="s">
+        <v>883</v>
+      </c>
+      <c r="B817" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="818" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A818" t="s">
+        <v>884</v>
+      </c>
+      <c r="B818" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A819" t="s">
+        <v>885</v>
+      </c>
+      <c r="B819" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A820" t="s">
+        <v>886</v>
+      </c>
+      <c r="B820" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A821" t="s">
+        <v>887</v>
+      </c>
+      <c r="B821" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A822" t="s">
+        <v>888</v>
+      </c>
+      <c r="B822" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="823" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A823" t="s">
+        <v>889</v>
+      </c>
+      <c r="B823" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A824" t="s">
+        <v>890</v>
+      </c>
+      <c r="B824" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A825" t="s">
+        <v>891</v>
+      </c>
+      <c r="B825" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A826" t="s">
+        <v>892</v>
+      </c>
+      <c r="B826" t="s">
+        <v>788</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>